<commit_message>
pdf Extraction code added
</commit_message>
<xml_diff>
--- a/Logs/Logs.xlsx
+++ b/Logs/Logs.xlsx
@@ -434,13 +434,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D196"/>
+  <dimension ref="A1:D199"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
     <col width="13.453125" customWidth="1" min="1" max="1"/>
     <col width="25.1796875" customWidth="1" min="2" max="2"/>
@@ -2981,15 +2981,53 @@
         </is>
       </c>
       <c r="B196" s="5" t="n">
-        <v>45030.43379539945</v>
+        <v>45030.43379540509</v>
       </c>
       <c r="C196" s="5" t="n">
-        <v>45030.43562432972</v>
+        <v>45030.4356243287</v>
       </c>
       <c r="D196" t="inlineStr">
         <is>
           <t>Task Completed</t>
         </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>Sachin.J</t>
+        </is>
+      </c>
+      <c r="B197" s="5" t="n">
+        <v>45030.48791054398</v>
+      </c>
+      <c r="C197" s="5" t="n">
+        <v>45030.48954752315</v>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>Task Completed</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>Sachin.J</t>
+        </is>
+      </c>
+      <c r="B198" s="5" t="n">
+        <v>45030.76237565972</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>Sachin.J</t>
+        </is>
+      </c>
+      <c r="B199" s="5" t="n">
+        <v>45030.76890122537</v>
       </c>
     </row>
   </sheetData>

</xml_diff>